<commit_message>
Actualización de código para formularios PIR.
</commit_message>
<xml_diff>
--- a/public/templates/pir001.xlsx
+++ b/public/templates/pir001.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="ALFA" sheetId="7" r:id="rId1"/>
-    <sheet name="BRAVO" sheetId="8" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ALFA!$A$1:$M$44</definedName>
@@ -612,16 +611,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,12 +728,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -761,6 +788,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -800,61 +830,34 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,12 +1355,12 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C26"/>
+      <selection activeCell="B12" sqref="B12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" style="1" customWidth="1"/>
     <col min="3" max="4" width="25.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="1"/>
@@ -1373,37 +1376,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="21">
-      <c r="C1" s="13"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="2:13" ht="23.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="49"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="46"/>
     </row>
     <row r="3" spans="2:13" ht="21">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="50"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="3"/>
@@ -1419,17 +1422,17 @@
       <c r="L4" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="18">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="4" t="s">
@@ -1458,17 +1461,17 @@
       </c>
     </row>
     <row r="9" spans="2:13">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="11" spans="2:13" ht="45">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1490,103 +1493,103 @@
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="92"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="59" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="38"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="38"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-    </row>
-    <row r="17" spans="1:13" s="20" customFormat="1" ht="15" customHeight="1">
-      <c r="A17" s="52" t="s">
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+    </row>
+    <row r="17" spans="1:13" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-    </row>
-    <row r="18" spans="1:13" s="20" customFormat="1" ht="30">
-      <c r="A18" s="53"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="54"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+    </row>
+    <row r="18" spans="1:13" s="17" customFormat="1" ht="30">
+      <c r="A18" s="57"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="5" t="s">
         <v>22</v>
       </c>
@@ -1607,99 +1610,99 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A19" s="48"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="35"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A20" s="47"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="35"/>
-    </row>
-    <row r="21" spans="1:13" s="14" customFormat="1" ht="21">
-      <c r="A21" s="27"/>
-      <c r="B21" s="70" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="32"/>
+    </row>
+    <row r="21" spans="1:13" s="11" customFormat="1" ht="21">
+      <c r="A21" s="24"/>
+      <c r="B21" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="85">
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="52">
         <f>COUNTIF(E19:E20,"X")</f>
         <v>0</v>
       </c>
-      <c r="F21" s="85">
+      <c r="F21" s="52">
         <f t="shared" ref="F21:H21" si="0">COUNTIF(F19:F20,"X")</f>
         <v>0</v>
       </c>
-      <c r="G21" s="85">
+      <c r="G21" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="85">
+      <c r="H21" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="21"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="28"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
     </row>
     <row r="23" spans="1:13" ht="15" customHeight="1">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="86" t="s">
+      <c r="C23" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
     </row>
     <row r="24" spans="1:13" ht="30">
-      <c r="A24" s="52"/>
-      <c r="B24" s="86"/>
-      <c r="C24" s="86"/>
-      <c r="D24" s="54"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1709,10 +1712,10 @@
       <c r="G24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I24" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J24" s="5" t="s">
@@ -1720,289 +1723,289 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="16.5">
-      <c r="A25" s="47"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="46"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="43"/>
     </row>
     <row r="26" spans="1:13" ht="16.5">
-      <c r="A26" s="47"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="46"/>
-    </row>
-    <row r="27" spans="1:13" s="14" customFormat="1" ht="21">
-      <c r="A27" s="27"/>
-      <c r="B27" s="70" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="88"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="43"/>
+    </row>
+    <row r="27" spans="1:13" s="11" customFormat="1" ht="21">
+      <c r="A27" s="24"/>
+      <c r="B27" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="71"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="85">
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="52">
         <f>COUNTIF(E25:E26,"X")</f>
         <v>0</v>
       </c>
-      <c r="F27" s="85">
+      <c r="F27" s="52">
         <f t="shared" ref="F27:H27" si="1">COUNTIF(F25:F26,"X")</f>
         <v>0</v>
       </c>
-      <c r="G27" s="85">
+      <c r="G27" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H27" s="85">
+      <c r="H27" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27" s="85"/>
-      <c r="J27" s="21"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="18">
-      <c r="A28" s="29"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="14"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="11"/>
     </row>
     <row r="29" spans="1:13" ht="18">
-      <c r="A29" s="29"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="14"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="11"/>
     </row>
     <row r="30" spans="1:13" ht="10.5" customHeight="1">
-      <c r="A30" s="29"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="14"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="11"/>
     </row>
     <row r="31" spans="1:13" ht="18">
-      <c r="A31" s="19"/>
-      <c r="B31" s="44" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="19" t="s">
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="L31" s="32"/>
-      <c r="M31" s="14"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="11"/>
     </row>
     <row r="32" spans="1:13" ht="18">
-      <c r="A32" s="19"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="14"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="11"/>
     </row>
     <row r="33" spans="1:13" ht="18.75" thickBot="1">
-      <c r="A33" s="19"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="14"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="11"/>
     </row>
     <row r="34" spans="1:13" ht="12.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="C34" s="61" t="s">
+      <c r="C34" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="63"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="30"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="27"/>
     </row>
     <row r="35" spans="1:13" ht="34.5" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="66"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="30"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="27"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="30"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="27"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="30"/>
+      <c r="C37" s="73"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="27"/>
     </row>
     <row r="38" spans="1:13" ht="21" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="65"/>
-      <c r="K38" s="66"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="30"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="27"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="30"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="27"/>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="66"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="30"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="75"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="27"/>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="65"/>
-      <c r="J41" s="65"/>
-      <c r="K41" s="66"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="30"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+      <c r="J41" s="74"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="27"/>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="30"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="75"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="27"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1">
       <c r="A43" s="1"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="30"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="77"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="77"/>
+      <c r="K43" s="78"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="23">
@@ -2034,18 +2037,4 @@
   <pageSetup scale="52" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>